<commit_message>
Linked FTTx Invoic to PO Excel
</commit_message>
<xml_diff>
--- a/input/Invoice/TNDSUMMARYMP01.xlsx
+++ b/input/Invoice/TNDSUMMARYMP01.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth.pandey\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth.pandey\Desktop\Automation\Code\input\Invoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29C892E-DB71-4DCB-A683-87734AA75577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50490852-03F1-4209-A162-FBB6350C58D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="772" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4048,92 +4048,75 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="48" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="31" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="25" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="25" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="32" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4168,6 +4151,12 @@
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4180,66 +4169,77 @@
     <xf numFmtId="172" fontId="25" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="31" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="48" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="31" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="32" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4277,24 +4277,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4307,6 +4289,24 @@
     <xf numFmtId="0" fontId="69" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4349,6 +4349,27 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4379,31 +4400,7 @@
     <xf numFmtId="0" fontId="57" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4412,6 +4409,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4428,9 +4431,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5030,193 +5030,193 @@
   <sheetData>
     <row r="6" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="7" spans="2:8" ht="23" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="532" t="s">
+      <c r="B7" s="488" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="533"/>
-      <c r="D7" s="534"/>
-      <c r="E7" s="534"/>
-      <c r="F7" s="534"/>
-      <c r="G7" s="534"/>
-      <c r="H7" s="535"/>
+      <c r="C7" s="489"/>
+      <c r="D7" s="490"/>
+      <c r="E7" s="490"/>
+      <c r="F7" s="490"/>
+      <c r="G7" s="490"/>
+      <c r="H7" s="491"/>
     </row>
     <row r="8" spans="2:8" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="536"/>
-      <c r="C8" s="537"/>
-      <c r="D8" s="538"/>
-      <c r="E8" s="538"/>
-      <c r="F8" s="538"/>
-      <c r="G8" s="538"/>
-      <c r="H8" s="539"/>
+      <c r="B8" s="492"/>
+      <c r="C8" s="493"/>
+      <c r="D8" s="494"/>
+      <c r="E8" s="494"/>
+      <c r="F8" s="494"/>
+      <c r="G8" s="494"/>
+      <c r="H8" s="495"/>
     </row>
     <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="491" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="493" t="s">
+      <c r="B9" s="535" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="537" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="493"/>
-      <c r="E9" s="494"/>
-      <c r="F9" s="540" t="s">
+      <c r="D9" s="537"/>
+      <c r="E9" s="538"/>
+      <c r="F9" s="496" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="542" t="s">
+      <c r="G9" s="498" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="543"/>
+      <c r="H9" s="499"/>
     </row>
     <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="492"/>
-      <c r="C10" s="495"/>
-      <c r="D10" s="495"/>
-      <c r="E10" s="496"/>
-      <c r="F10" s="541"/>
-      <c r="G10" s="544"/>
-      <c r="H10" s="545"/>
+      <c r="B10" s="536"/>
+      <c r="C10" s="539"/>
+      <c r="D10" s="539"/>
+      <c r="E10" s="540"/>
+      <c r="F10" s="497"/>
+      <c r="G10" s="500"/>
+      <c r="H10" s="501"/>
     </row>
     <row r="11" spans="2:8" s="30" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="546" t="s">
+      <c r="B11" s="502" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="547"/>
-      <c r="D11" s="548" t="s">
+      <c r="C11" s="503"/>
+      <c r="D11" s="504" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="549" t="s">
+      <c r="E11" s="505" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="541"/>
-      <c r="G11" s="544"/>
-      <c r="H11" s="545"/>
+      <c r="F11" s="497"/>
+      <c r="G11" s="500"/>
+      <c r="H11" s="501"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="517" t="s">
+      <c r="B12" s="510" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="518"/>
-      <c r="D12" s="519"/>
-      <c r="E12" s="520"/>
+      <c r="C12" s="511"/>
+      <c r="D12" s="512"/>
+      <c r="E12" s="513"/>
       <c r="F12" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="521" t="str">
+      <c r="G12" s="514" t="str">
         <f>+'QCS '!F3</f>
         <v>TNDMNETMP01-3</v>
       </c>
-      <c r="H12" s="522"/>
+      <c r="H12" s="515"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="31"/>
-      <c r="C13" s="523" t="s">
+      <c r="C13" s="516" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="524" t="s">
+      <c r="D13" s="517" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="525" t="s">
+      <c r="E13" s="518" t="s">
         <v>57</v>
       </c>
       <c r="F13" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="526">
+      <c r="G13" s="519">
         <v>44534</v>
       </c>
-      <c r="H13" s="522"/>
+      <c r="H13" s="515"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="31"/>
-      <c r="C14" s="524" t="s">
+      <c r="C14" s="517" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="524" t="s">
+      <c r="D14" s="517" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="525" t="s">
+      <c r="E14" s="518" t="s">
         <v>60</v>
       </c>
       <c r="F14" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="511" t="str">
+      <c r="G14" s="520" t="str">
         <f>+'QCS '!D2</f>
         <v>P11/630098168</v>
       </c>
-      <c r="H14" s="512"/>
+      <c r="H14" s="521"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" s="32"/>
-      <c r="C15" s="527" t="s">
+      <c r="C15" s="522" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="527" t="s">
+      <c r="D15" s="522" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="528" t="s">
+      <c r="E15" s="523" t="s">
         <v>62</v>
       </c>
       <c r="F15" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="529">
+      <c r="G15" s="524">
         <f>+'QCS '!D3</f>
         <v>44417</v>
       </c>
-      <c r="H15" s="530"/>
+      <c r="H15" s="525"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="507" t="s">
+      <c r="B16" s="526" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="531"/>
-      <c r="D16" s="509" t="s">
+      <c r="C16" s="527"/>
+      <c r="D16" s="528" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="510" t="s">
+      <c r="E16" s="529" t="s">
         <v>65</v>
       </c>
       <c r="F16" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="G16" s="501" t="str">
+      <c r="G16" s="508" t="str">
         <f>+'OT SUMMARY'!D10</f>
         <v>MUMB0309</v>
       </c>
-      <c r="H16" s="502"/>
+      <c r="H16" s="509"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="33"/>
       <c r="C17" s="34"/>
-      <c r="D17" s="515"/>
-      <c r="E17" s="516"/>
+      <c r="D17" s="506"/>
+      <c r="E17" s="507"/>
       <c r="F17" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="G17" s="501" t="str">
+      <c r="G17" s="508" t="str">
         <f>+'OT SUMMARY'!B10</f>
         <v>KONARK</v>
       </c>
-      <c r="H17" s="502"/>
+      <c r="H17" s="509"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B18" s="507" t="s">
+      <c r="B18" s="526" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="508"/>
-      <c r="D18" s="509" t="s">
+      <c r="C18" s="549"/>
+      <c r="D18" s="528" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="510" t="s">
+      <c r="E18" s="529" t="s">
         <v>66</v>
       </c>
       <c r="F18" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="511" t="s">
+      <c r="G18" s="520" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="512" t="s">
+      <c r="H18" s="521" t="s">
         <v>68</v>
       </c>
     </row>
@@ -5228,31 +5228,31 @@
       <c r="F19" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="511" t="s">
+      <c r="G19" s="520" t="s">
         <v>69</v>
       </c>
-      <c r="H19" s="512" t="s">
+      <c r="H19" s="521" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B20" s="513" t="s">
+      <c r="B20" s="530" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="514"/>
-      <c r="D20" s="509" t="s">
+      <c r="C20" s="531"/>
+      <c r="D20" s="528" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="510" t="s">
+      <c r="E20" s="529" t="s">
         <v>70</v>
       </c>
       <c r="F20" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="511" t="s">
+      <c r="G20" s="520" t="s">
         <v>71</v>
       </c>
-      <c r="H20" s="512" t="s">
+      <c r="H20" s="521" t="s">
         <v>71</v>
       </c>
     </row>
@@ -5264,11 +5264,11 @@
       <c r="F21" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="G21" s="501" t="str">
+      <c r="G21" s="508" t="str">
         <f>+'QCS '!D4</f>
         <v>12-02-2021 To 12-02-2021</v>
       </c>
-      <c r="H21" s="502"/>
+      <c r="H21" s="509"/>
     </row>
     <row r="22" spans="2:8" s="30" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B22" s="37"/>
@@ -5278,10 +5278,10 @@
       <c r="F22" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="G22" s="503" t="s">
+      <c r="G22" s="545" t="s">
         <v>74</v>
       </c>
-      <c r="H22" s="504" t="s">
+      <c r="H22" s="546" t="s">
         <v>74</v>
       </c>
     </row>
@@ -5293,10 +5293,10 @@
       <c r="F23" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="G23" s="505" t="s">
+      <c r="G23" s="547" t="s">
         <v>76</v>
       </c>
-      <c r="H23" s="506" t="s">
+      <c r="H23" s="548" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5542,10 +5542,10 @@
       <c r="C35" s="49"/>
       <c r="D35" s="52"/>
       <c r="E35" s="53"/>
-      <c r="F35" s="497" t="s">
+      <c r="F35" s="541" t="s">
         <v>80</v>
       </c>
-      <c r="G35" s="497"/>
+      <c r="G35" s="541"/>
       <c r="H35" s="100">
         <f>H34*9%</f>
         <v>8932.6332000000002</v>
@@ -5556,10 +5556,10 @@
       <c r="C36" s="49"/>
       <c r="D36" s="52"/>
       <c r="E36" s="53"/>
-      <c r="F36" s="497" t="s">
+      <c r="F36" s="541" t="s">
         <v>81</v>
       </c>
-      <c r="G36" s="497"/>
+      <c r="G36" s="541"/>
       <c r="H36" s="100">
         <f>H34*9%</f>
         <v>8932.6332000000002</v>
@@ -5570,10 +5570,10 @@
       <c r="C37" s="51"/>
       <c r="D37" s="52"/>
       <c r="E37" s="53"/>
-      <c r="F37" s="497" t="s">
+      <c r="F37" s="541" t="s">
         <v>82</v>
       </c>
-      <c r="G37" s="497"/>
+      <c r="G37" s="541"/>
       <c r="H37" s="102">
         <f>H35+H36</f>
         <v>17865.2664</v>
@@ -5584,10 +5584,10 @@
       <c r="C38" s="51"/>
       <c r="D38" s="52"/>
       <c r="E38" s="53"/>
-      <c r="F38" s="497" t="s">
+      <c r="F38" s="541" t="s">
         <v>83</v>
       </c>
-      <c r="G38" s="497"/>
+      <c r="G38" s="541"/>
       <c r="H38" s="100">
         <f>H34+H37</f>
         <v>117116.7464</v>
@@ -5598,10 +5598,10 @@
       <c r="C39" s="51"/>
       <c r="D39" s="52"/>
       <c r="E39" s="53"/>
-      <c r="F39" s="497" t="s">
+      <c r="F39" s="541" t="s">
         <v>84</v>
       </c>
-      <c r="G39" s="497"/>
+      <c r="G39" s="541"/>
       <c r="H39" s="100">
         <v>0</v>
       </c>
@@ -5611,24 +5611,24 @@
       <c r="C40" s="51"/>
       <c r="D40" s="52"/>
       <c r="E40" s="53"/>
-      <c r="F40" s="497" t="s">
+      <c r="F40" s="541" t="s">
         <v>85</v>
       </c>
-      <c r="G40" s="497"/>
+      <c r="G40" s="541"/>
       <c r="H40" s="101">
         <f>H38</f>
         <v>117116.7464</v>
       </c>
     </row>
     <row r="41" spans="2:8" s="30" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B41" s="498"/>
-      <c r="C41" s="499"/>
-      <c r="D41" s="499"/>
+      <c r="B41" s="542"/>
+      <c r="C41" s="543"/>
+      <c r="D41" s="543"/>
       <c r="E41" s="53"/>
-      <c r="F41" s="500" t="s">
+      <c r="F41" s="544" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="500"/>
+      <c r="G41" s="544"/>
       <c r="H41" s="103">
         <f>ROUNDUP(H40,0)</f>
         <v>117117</v>
@@ -5647,27 +5647,27 @@
       <c r="B43" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="488" t="s">
+      <c r="C43" s="532" t="s">
         <v>295</v>
       </c>
-      <c r="D43" s="489"/>
-      <c r="E43" s="489"/>
-      <c r="F43" s="489"/>
-      <c r="G43" s="489"/>
-      <c r="H43" s="490"/>
+      <c r="D43" s="533"/>
+      <c r="E43" s="533"/>
+      <c r="F43" s="533"/>
+      <c r="G43" s="533"/>
+      <c r="H43" s="534"/>
     </row>
     <row r="44" spans="2:8" s="30" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B44" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="488" t="s">
+      <c r="C44" s="532" t="s">
         <v>296</v>
       </c>
-      <c r="D44" s="489"/>
-      <c r="E44" s="489"/>
-      <c r="F44" s="489"/>
-      <c r="G44" s="489"/>
-      <c r="H44" s="490"/>
+      <c r="D44" s="533"/>
+      <c r="E44" s="533"/>
+      <c r="F44" s="533"/>
+      <c r="G44" s="533"/>
+      <c r="H44" s="534"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45" s="55"/>
@@ -5760,32 +5760,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:H11"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="G20:H20"/>
     <mergeCell ref="C43:H43"/>
     <mergeCell ref="C44:H44"/>
     <mergeCell ref="B9:B10"/>
@@ -5802,6 +5776,32 @@
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="F35:G35"/>
     <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:H11"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
   </mergeCells>
   <pageMargins left="0.38" right="0.24" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="63" orientation="portrait" r:id="rId1"/>
@@ -8278,13 +8278,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
-    <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11166,70 +11165,70 @@
       <c r="O7" s="453"/>
     </row>
     <row r="8" spans="1:20" s="454" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="562" t="s">
+      <c r="A8" s="566" t="s">
         <v>251</v>
       </c>
-      <c r="B8" s="564" t="s">
+      <c r="B8" s="568" t="s">
         <v>252</v>
       </c>
       <c r="C8" s="572" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="566" t="s">
+      <c r="D8" s="570" t="s">
         <v>253</v>
       </c>
-      <c r="E8" s="566" t="s">
+      <c r="E8" s="570" t="s">
         <v>254</v>
       </c>
-      <c r="F8" s="568" t="s">
+      <c r="F8" s="562" t="s">
         <v>282</v>
       </c>
-      <c r="G8" s="568"/>
-      <c r="H8" s="568" t="s">
+      <c r="G8" s="562"/>
+      <c r="H8" s="562" t="s">
         <v>255</v>
       </c>
-      <c r="I8" s="568" t="s">
+      <c r="I8" s="562" t="s">
         <v>256</v>
       </c>
-      <c r="J8" s="568" t="s">
+      <c r="J8" s="562" t="s">
         <v>257</v>
       </c>
-      <c r="K8" s="568" t="s">
+      <c r="K8" s="562" t="s">
         <v>269</v>
       </c>
-      <c r="L8" s="568" t="s">
+      <c r="L8" s="562" t="s">
         <v>283</v>
       </c>
-      <c r="M8" s="568" t="s">
+      <c r="M8" s="562" t="s">
         <v>271</v>
       </c>
-      <c r="N8" s="568" t="s">
+      <c r="N8" s="562" t="s">
         <v>258</v>
       </c>
-      <c r="O8" s="570" t="s">
+      <c r="O8" s="564" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="454" customFormat="1" ht="37.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="563"/>
-      <c r="B9" s="565"/>
+      <c r="A9" s="567"/>
+      <c r="B9" s="569"/>
       <c r="C9" s="573"/>
-      <c r="D9" s="567"/>
-      <c r="E9" s="567"/>
+      <c r="D9" s="571"/>
+      <c r="E9" s="571"/>
       <c r="F9" s="455" t="s">
         <v>260</v>
       </c>
       <c r="G9" s="456" t="s">
         <v>261</v>
       </c>
-      <c r="H9" s="569"/>
-      <c r="I9" s="569"/>
-      <c r="J9" s="569"/>
-      <c r="K9" s="569"/>
-      <c r="L9" s="569"/>
-      <c r="M9" s="569"/>
-      <c r="N9" s="569"/>
-      <c r="O9" s="571"/>
+      <c r="H9" s="563"/>
+      <c r="I9" s="563"/>
+      <c r="J9" s="563"/>
+      <c r="K9" s="563"/>
+      <c r="L9" s="563"/>
+      <c r="M9" s="563"/>
+      <c r="N9" s="563"/>
+      <c r="O9" s="565"/>
     </row>
     <row r="10" spans="1:20" s="464" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="457" t="s">
@@ -11514,6 +11513,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="C8:C9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="J8:J9"/>
@@ -11522,12 +11527,6 @@
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="N8:N9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="C8:C9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.15748031496062992" right="0.19685039370078741" top="0.27559055118110237" bottom="0.35433070866141736" header="0.15748031496062992" footer="0.31496062992125984"/>
@@ -11939,44 +11938,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="586" t="s">
+      <c r="A1" s="593" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="586"/>
-      <c r="C1" s="586"/>
-      <c r="D1" s="586"/>
-      <c r="E1" s="586"/>
-      <c r="F1" s="586"/>
-      <c r="G1" s="586"/>
-      <c r="H1" s="586"/>
-      <c r="I1" s="586"/>
-      <c r="J1" s="586"/>
-      <c r="K1" s="586"/>
-      <c r="L1" s="586"/>
-      <c r="M1" s="586"/>
-      <c r="N1" s="586"/>
-      <c r="O1" s="586"/>
-      <c r="P1" s="586"/>
+      <c r="B1" s="593"/>
+      <c r="C1" s="593"/>
+      <c r="D1" s="593"/>
+      <c r="E1" s="593"/>
+      <c r="F1" s="593"/>
+      <c r="G1" s="593"/>
+      <c r="H1" s="593"/>
+      <c r="I1" s="593"/>
+      <c r="J1" s="593"/>
+      <c r="K1" s="593"/>
+      <c r="L1" s="593"/>
+      <c r="M1" s="593"/>
+      <c r="N1" s="593"/>
+      <c r="O1" s="593"/>
+      <c r="P1" s="593"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="587" t="s">
+      <c r="A2" s="594" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="587"/>
-      <c r="C2" s="587"/>
-      <c r="D2" s="587"/>
-      <c r="E2" s="587"/>
-      <c r="F2" s="587"/>
-      <c r="G2" s="587"/>
-      <c r="H2" s="587"/>
-      <c r="I2" s="587"/>
-      <c r="J2" s="587"/>
-      <c r="K2" s="587"/>
-      <c r="L2" s="587"/>
-      <c r="M2" s="587"/>
-      <c r="N2" s="587"/>
-      <c r="O2" s="587"/>
-      <c r="P2" s="587"/>
+      <c r="B2" s="594"/>
+      <c r="C2" s="594"/>
+      <c r="D2" s="594"/>
+      <c r="E2" s="594"/>
+      <c r="F2" s="594"/>
+      <c r="G2" s="594"/>
+      <c r="H2" s="594"/>
+      <c r="I2" s="594"/>
+      <c r="J2" s="594"/>
+      <c r="K2" s="594"/>
+      <c r="L2" s="594"/>
+      <c r="M2" s="594"/>
+      <c r="N2" s="594"/>
+      <c r="O2" s="594"/>
+      <c r="P2" s="594"/>
     </row>
     <row r="3" spans="1:16" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A3" s="255"/>
@@ -11984,12 +11983,12 @@
         <v>48</v>
       </c>
       <c r="C3" s="20"/>
-      <c r="D3" s="598" t="str">
+      <c r="D3" s="588" t="str">
         <f>+Manhole!C2</f>
         <v>MP 01 (MCGM)</v>
       </c>
-      <c r="E3" s="599"/>
-      <c r="F3" s="600"/>
+      <c r="E3" s="589"/>
+      <c r="F3" s="590"/>
       <c r="G3" s="260"/>
       <c r="H3" s="260"/>
       <c r="I3" s="261"/>
@@ -12048,10 +12047,10 @@
     </row>
     <row r="6" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="255"/>
-      <c r="B6" s="601" t="s">
+      <c r="B6" s="591" t="s">
         <v>148</v>
       </c>
-      <c r="C6" s="602"/>
+      <c r="C6" s="592"/>
       <c r="D6" s="585" t="str">
         <f>+Manhole!C5</f>
         <v>TNDMNETMP01-3</v>
@@ -12129,27 +12128,27 @@
       <c r="P9" s="260"/>
     </row>
     <row r="10" spans="1:16" s="271" customFormat="1" ht="24.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="588" t="s">
+      <c r="A10" s="595" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="590" t="s">
+      <c r="B10" s="597" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="590" t="s">
+      <c r="C10" s="597" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="592" t="s">
+      <c r="D10" s="599" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="592"/>
-      <c r="F10" s="592" t="s">
+      <c r="E10" s="599"/>
+      <c r="F10" s="599" t="s">
         <v>158</v>
       </c>
-      <c r="G10" s="592"/>
+      <c r="G10" s="599"/>
       <c r="H10" s="268" t="s">
         <v>159</v>
       </c>
-      <c r="I10" s="593" t="s">
+      <c r="I10" s="600" t="s">
         <v>238</v>
       </c>
       <c r="J10" s="269" t="s">
@@ -12164,20 +12163,20 @@
       <c r="M10" s="270" t="s">
         <v>162</v>
       </c>
-      <c r="N10" s="593" t="s">
+      <c r="N10" s="600" t="s">
         <v>163</v>
       </c>
-      <c r="O10" s="595" t="s">
+      <c r="O10" s="602" t="s">
         <v>164</v>
       </c>
-      <c r="P10" s="595" t="s">
+      <c r="P10" s="602" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="271" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="589"/>
-      <c r="B11" s="591"/>
-      <c r="C11" s="591"/>
+      <c r="A11" s="596"/>
+      <c r="B11" s="598"/>
+      <c r="C11" s="598"/>
       <c r="D11" s="272" t="s">
         <v>30</v>
       </c>
@@ -12193,7 +12192,7 @@
       <c r="H11" s="268" t="s">
         <v>100</v>
       </c>
-      <c r="I11" s="594"/>
+      <c r="I11" s="601"/>
       <c r="J11" s="274" t="s">
         <v>165</v>
       </c>
@@ -12206,9 +12205,9 @@
       <c r="M11" s="273" t="s">
         <v>166</v>
       </c>
-      <c r="N11" s="594"/>
-      <c r="O11" s="595"/>
-      <c r="P11" s="595"/>
+      <c r="N11" s="601"/>
+      <c r="O11" s="602"/>
+      <c r="P11" s="602"/>
     </row>
     <row r="12" spans="1:16" s="271" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="275"/>
@@ -12472,10 +12471,10 @@
     <row r="21" spans="1:18" s="305" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="301"/>
       <c r="B21" s="262"/>
-      <c r="C21" s="596" t="s">
+      <c r="C21" s="586" t="s">
         <v>175</v>
       </c>
-      <c r="D21" s="597"/>
+      <c r="D21" s="587"/>
       <c r="E21" s="302">
         <f>+N19</f>
         <v>0</v>
@@ -12496,10 +12495,10 @@
     <row r="22" spans="1:18" s="305" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="301"/>
       <c r="B22" s="262"/>
-      <c r="C22" s="596" t="s">
+      <c r="C22" s="586" t="s">
         <v>176</v>
       </c>
-      <c r="D22" s="597"/>
+      <c r="D22" s="587"/>
       <c r="E22" s="302">
         <v>0</v>
       </c>
@@ -12518,10 +12517,10 @@
     </row>
     <row r="23" spans="1:18" s="305" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="B23" s="306"/>
-      <c r="C23" s="596" t="s">
+      <c r="C23" s="586" t="s">
         <v>177</v>
       </c>
-      <c r="D23" s="597"/>
+      <c r="D23" s="587"/>
       <c r="E23" s="302">
         <f>+O19</f>
         <v>0</v>
@@ -12546,15 +12545,6 @@
   </sheetData>
   <autoFilter ref="A12:P19" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
   <mergeCells count="20">
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="C21:D21"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:P2"/>
     <mergeCell ref="A10:A11"/>
@@ -12566,6 +12556,15 @@
     <mergeCell ref="N10:N11"/>
     <mergeCell ref="O10:O11"/>
     <mergeCell ref="P10:P11"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.55118110236220474" bottom="0.51181102362204722" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -12630,11 +12629,11 @@
         <v>237</v>
       </c>
       <c r="C2" s="20"/>
-      <c r="D2" s="598" t="s">
+      <c r="D2" s="588" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="599"/>
-      <c r="F2" s="600"/>
+      <c r="E2" s="589"/>
+      <c r="F2" s="590"/>
       <c r="G2" s="28"/>
       <c r="H2" s="28"/>
       <c r="I2" s="28"/>
@@ -12652,12 +12651,12 @@
         <v>48</v>
       </c>
       <c r="C3" s="20"/>
-      <c r="D3" s="598" t="str">
+      <c r="D3" s="588" t="str">
         <f>+'Blowing Ribbon'!D3:F3</f>
         <v>MP 01 (MCGM)</v>
       </c>
-      <c r="E3" s="599"/>
-      <c r="F3" s="600"/>
+      <c r="E3" s="589"/>
+      <c r="F3" s="590"/>
       <c r="G3" s="28"/>
       <c r="H3" s="28"/>
       <c r="I3" s="28"/>
@@ -12716,16 +12715,16 @@
     </row>
     <row r="6" spans="1:16" s="157" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="314"/>
-      <c r="B6" s="601" t="s">
+      <c r="B6" s="591" t="s">
         <v>148</v>
       </c>
-      <c r="C6" s="602"/>
-      <c r="D6" s="598" t="str">
+      <c r="C6" s="592"/>
+      <c r="D6" s="588" t="str">
         <f>+'Blowing Ribbon'!D6:F6</f>
         <v>TNDMNETMP01-3</v>
       </c>
-      <c r="E6" s="599"/>
-      <c r="F6" s="600"/>
+      <c r="E6" s="589"/>
+      <c r="F6" s="590"/>
       <c r="G6" s="250"/>
       <c r="H6" s="317"/>
       <c r="I6" s="318"/>
@@ -12743,12 +12742,12 @@
         <v>51</v>
       </c>
       <c r="C7" s="25"/>
-      <c r="D7" s="598" t="str">
+      <c r="D7" s="588" t="str">
         <f>+'Blowing Ribbon'!D7:F7</f>
         <v>12-02-2021 To 12-02-2021</v>
       </c>
-      <c r="E7" s="599"/>
-      <c r="F7" s="600"/>
+      <c r="E7" s="589"/>
+      <c r="F7" s="590"/>
       <c r="G7" s="250"/>
       <c r="H7" s="317"/>
       <c r="I7" s="318"/>
@@ -12779,56 +12778,56 @@
       <c r="P8" s="319"/>
     </row>
     <row r="9" spans="1:16" s="146" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="609" t="s">
+      <c r="A9" s="610" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="611" t="s">
+      <c r="B9" s="612" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="611" t="s">
+      <c r="C9" s="612" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="611" t="s">
+      <c r="D9" s="612" t="s">
         <v>178</v>
       </c>
-      <c r="E9" s="611" t="s">
+      <c r="E9" s="612" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="611" t="s">
+      <c r="F9" s="612" t="s">
         <v>179</v>
       </c>
-      <c r="G9" s="605" t="s">
+      <c r="G9" s="604" t="s">
         <v>180</v>
       </c>
-      <c r="H9" s="605" t="s">
+      <c r="H9" s="604" t="s">
         <v>181</v>
       </c>
-      <c r="I9" s="603" t="s">
+      <c r="I9" s="606" t="s">
         <v>182</v>
       </c>
-      <c r="J9" s="603"/>
-      <c r="K9" s="604"/>
-      <c r="L9" s="603" t="s">
+      <c r="J9" s="606"/>
+      <c r="K9" s="607"/>
+      <c r="L9" s="606" t="s">
         <v>183</v>
       </c>
-      <c r="M9" s="603"/>
-      <c r="N9" s="604"/>
-      <c r="O9" s="605" t="s">
+      <c r="M9" s="606"/>
+      <c r="N9" s="607"/>
+      <c r="O9" s="604" t="s">
         <v>184</v>
       </c>
-      <c r="P9" s="607" t="s">
+      <c r="P9" s="608" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="146" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="610"/>
-      <c r="B10" s="612"/>
-      <c r="C10" s="612"/>
-      <c r="D10" s="612"/>
-      <c r="E10" s="612"/>
-      <c r="F10" s="612"/>
-      <c r="G10" s="606"/>
-      <c r="H10" s="606"/>
+      <c r="A10" s="611"/>
+      <c r="B10" s="613"/>
+      <c r="C10" s="613"/>
+      <c r="D10" s="613"/>
+      <c r="E10" s="613"/>
+      <c r="F10" s="613"/>
+      <c r="G10" s="605"/>
+      <c r="H10" s="605"/>
       <c r="I10" s="91">
         <v>48</v>
       </c>
@@ -12847,8 +12846,8 @@
       <c r="N10" s="91">
         <v>288</v>
       </c>
-      <c r="O10" s="606"/>
-      <c r="P10" s="608"/>
+      <c r="O10" s="605"/>
+      <c r="P10" s="609"/>
     </row>
     <row r="11" spans="1:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="323"/>
@@ -13073,12 +13072,12 @@
       <c r="D20" s="345" t="s">
         <v>188</v>
       </c>
-      <c r="E20" s="613" t="s">
+      <c r="E20" s="603" t="s">
         <v>239</v>
       </c>
-      <c r="F20" s="613"/>
-      <c r="G20" s="613"/>
-      <c r="H20" s="613"/>
+      <c r="F20" s="603"/>
+      <c r="G20" s="603"/>
+      <c r="H20" s="603"/>
       <c r="I20" s="345" t="s">
         <v>78</v>
       </c>
@@ -13552,6 +13551,16 @@
   </sheetData>
   <autoFilter ref="A11:P31" xr:uid="{00000000-0009-0000-0000-000009000000}"/>
   <mergeCells count="20">
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="D7:F7"/>
@@ -13562,16 +13571,6 @@
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35433070866141736" right="0.15748031496062992" top="1.36" bottom="1.29" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>